<commit_message>
Agregando archivos por ciudades
</commit_message>
<xml_diff>
--- a/Siati/plantilla_inventario.xlsx
+++ b/Siati/plantilla_inventario.xlsx
@@ -468,7 +468,7 @@
     <numFmt numFmtId="169" formatCode="h:mm"/>
     <numFmt numFmtId="170" formatCode="[$-C0A]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -556,13 +556,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="20"/>
       <name val="Arial"/>
@@ -578,12 +571,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -605,6 +592,13 @@
       <b val="true"/>
       <i val="true"/>
       <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -788,7 +782,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1154,6 +1148,17 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="thin"/>
+      <top style="thin">
+        <color theme="0" tint="-0.35"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.35"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -1163,7 +1168,7 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
+      <right style="thin"/>
       <top style="thin">
         <color theme="0" tint="-0.35"/>
       </top>
@@ -1239,7 +1244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="180">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1325,42 +1330,34 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1376,19 +1373,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1396,7 +1393,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1404,16 +1401,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1424,7 +1413,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1436,7 +1425,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1444,11 +1433,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1460,11 +1449,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1484,7 +1473,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1504,7 +1493,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1532,47 +1521,47 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1616,7 +1605,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1624,111 +1617,111 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1736,47 +1729,47 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="31" fillId="3" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="32" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="32" fillId="3" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="31" fillId="3" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1784,11 +1777,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1796,7 +1789,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1804,15 +1797,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1840,11 +1833,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1868,95 +1861,95 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1964,7 +1957,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2055,9 +2048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2099520</xdr:colOff>
+      <xdr:colOff>2098440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>323640</xdr:rowOff>
+      <xdr:rowOff>322560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2072,7 +2065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="402840" y="52560"/>
-          <a:ext cx="3005280" cy="928440"/>
+          <a:ext cx="3004200" cy="927360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2098,9 +2091,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1361160</xdr:colOff>
+      <xdr:colOff>1360080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>102600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2115,7 +2108,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="123840" y="47520"/>
-          <a:ext cx="1982880" cy="551520"/>
+          <a:ext cx="1981800" cy="550440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2309,8 +2302,8 @@
   </sheetPr>
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q55" activeCellId="0" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2493,45 +2486,45 @@
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="24" t="s">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="27"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="25"/>
       <c r="T7" s="14"/>
     </row>
     <row r="8" s="15" customFormat="true" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="33"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="31"/>
       <c r="T8" s="14"/>
     </row>
     <row r="9" s="15" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2540,46 +2533,46 @@
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="24" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="36"/>
-      <c r="S9" s="37"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="35"/>
       <c r="T9" s="14"/>
     </row>
     <row r="10" s="15" customFormat="true" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
-      <c r="S10" s="38"/>
+      <c r="S10" s="36"/>
       <c r="T10" s="14"/>
     </row>
     <row r="11" s="15" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2588,30 +2581,30 @@
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="40" t="s">
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="43"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
       <c r="T11" s="14"/>
     </row>
     <row r="12" s="15" customFormat="true" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2628,45 +2621,45 @@
       <c r="T12" s="14"/>
     </row>
     <row r="13" s="15" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="E13" s="46" t="s">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="E13" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="46" t="s">
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="46"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="49" t="s">
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="49"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="50"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="46"/>
       <c r="T13" s="14"/>
     </row>
     <row r="14" s="15" customFormat="true" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="14"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
@@ -2674,37 +2667,37 @@
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
-      <c r="S14" s="38"/>
+      <c r="S14" s="36"/>
       <c r="T14" s="14"/>
     </row>
     <row r="15" s="15" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="55"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="14"/>
-      <c r="J15" s="46" t="s">
+      <c r="J15" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="46"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="33"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="31"/>
       <c r="T15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="57"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="11"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2722,36 +2715,36 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="58"/>
+      <c r="S16" s="54"/>
       <c r="T16" s="6"/>
     </row>
     <row r="17" s="15" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="59"/>
-      <c r="S17" s="59"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="55"/>
       <c r="T17" s="14"/>
     </row>
     <row r="18" s="15" customFormat="true" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -2772,451 +2765,451 @@
       <c r="T18" s="14"/>
     </row>
     <row r="19" s="15" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="61"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="57"/>
+      <c r="S19" s="57"/>
       <c r="T19" s="14"/>
     </row>
     <row r="20" s="15" customFormat="true" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="59" t="s">
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="62" t="s">
+      <c r="H20" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62" t="s">
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62" t="s">
+      <c r="L20" s="58"/>
+      <c r="M20" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62" t="s">
+      <c r="N20" s="58"/>
+      <c r="O20" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62" t="s">
+      <c r="P20" s="58"/>
+      <c r="Q20" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
       <c r="T20" s="14"/>
     </row>
     <row r="21" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="63" t="n">
+      <c r="A21" s="59" t="n">
         <v>1</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="65"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="66"/>
-      <c r="S21" s="66"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="61"/>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="62"/>
       <c r="T21" s="14"/>
     </row>
     <row r="22" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="63" t="n">
+      <c r="A22" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
-      <c r="N22" s="64"/>
-      <c r="O22" s="65"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
-      <c r="S22" s="66"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="61"/>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="62"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="62"/>
       <c r="T22" s="14"/>
     </row>
     <row r="23" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="63" t="n">
+      <c r="A23" s="59" t="n">
         <v>3</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="65"/>
-      <c r="P23" s="65"/>
-      <c r="Q23" s="66"/>
-      <c r="R23" s="66"/>
-      <c r="S23" s="66"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
       <c r="T23" s="14"/>
     </row>
     <row r="24" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="63" t="n">
+      <c r="A24" s="59" t="n">
         <v>4</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="65"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="66"/>
-      <c r="R24" s="66"/>
-      <c r="S24" s="66"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="62"/>
+      <c r="R24" s="62"/>
+      <c r="S24" s="62"/>
       <c r="T24" s="14"/>
     </row>
     <row r="25" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="63" t="n">
+      <c r="A25" s="59" t="n">
         <v>5</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="65"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="66"/>
-      <c r="R25" s="66"/>
-      <c r="S25" s="66"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
+      <c r="S25" s="62"/>
       <c r="T25" s="14"/>
     </row>
     <row r="26" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="63" t="n">
+      <c r="A26" s="59" t="n">
         <v>6</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="64"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="66"/>
-      <c r="R26" s="66"/>
-      <c r="S26" s="66"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="61"/>
+      <c r="Q26" s="62"/>
+      <c r="R26" s="62"/>
+      <c r="S26" s="62"/>
       <c r="T26" s="14"/>
     </row>
     <row r="27" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="63" t="n">
+      <c r="A27" s="59" t="n">
         <v>7</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="66"/>
-      <c r="R27" s="66"/>
-      <c r="S27" s="66"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
       <c r="T27" s="14"/>
     </row>
     <row r="28" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="63" t="n">
+      <c r="A28" s="59" t="n">
         <v>8</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="65"/>
-      <c r="P28" s="65"/>
-      <c r="Q28" s="66"/>
-      <c r="R28" s="66"/>
-      <c r="S28" s="66"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="62"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="62"/>
       <c r="T28" s="14"/>
     </row>
     <row r="29" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="63" t="n">
+      <c r="A29" s="59" t="n">
         <v>9</v>
       </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="65"/>
-      <c r="P29" s="65"/>
-      <c r="Q29" s="66"/>
-      <c r="R29" s="66"/>
-      <c r="S29" s="66"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="62"/>
+      <c r="R29" s="62"/>
+      <c r="S29" s="62"/>
       <c r="T29" s="14"/>
     </row>
     <row r="30" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="63" t="n">
+      <c r="A30" s="59" t="n">
         <v>10</v>
       </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-      <c r="O30" s="65"/>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="66"/>
-      <c r="R30" s="66"/>
-      <c r="S30" s="66"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="61"/>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="62"/>
+      <c r="R30" s="62"/>
+      <c r="S30" s="62"/>
       <c r="T30" s="14"/>
     </row>
     <row r="31" s="15" customFormat="true" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="63" t="n">
+      <c r="A31" s="59" t="n">
         <v>11</v>
       </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="65"/>
-      <c r="P31" s="65"/>
-      <c r="Q31" s="66"/>
-      <c r="R31" s="66"/>
-      <c r="S31" s="66"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="61"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="62"/>
+      <c r="S31" s="62"/>
       <c r="T31" s="14"/>
     </row>
     <row r="32" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="67"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="71"/>
-      <c r="N32" s="71"/>
-      <c r="O32" s="71"/>
-      <c r="P32" s="71"/>
-      <c r="Q32" s="72"/>
-      <c r="R32" s="72"/>
-      <c r="S32" s="72"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="68"/>
+      <c r="R32" s="68"/>
+      <c r="S32" s="68"/>
       <c r="T32" s="14"/>
     </row>
-    <row r="33" s="81" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="73" t="s">
+    <row r="33" s="77" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="75"/>
-      <c r="P33" s="76"/>
-      <c r="Q33" s="77"/>
-      <c r="R33" s="78"/>
-      <c r="S33" s="79"/>
-      <c r="T33" s="80"/>
-    </row>
-    <row r="34" s="81" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="73" t="s">
+      <c r="B33" s="69"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="72"/>
+      <c r="Q33" s="73"/>
+      <c r="R33" s="74"/>
+      <c r="S33" s="75"/>
+      <c r="T33" s="76"/>
+    </row>
+    <row r="34" s="77" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="46" t="s">
+      <c r="B34" s="69"/>
+      <c r="C34" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="74"/>
-      <c r="O34" s="74"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="74"/>
-      <c r="S34" s="74"/>
-      <c r="T34" s="80"/>
-    </row>
-    <row r="35" s="81" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="82" t="s">
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="76"/>
+    </row>
+    <row r="35" s="77" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="82"/>
-      <c r="C35" s="83" t="s">
+      <c r="B35" s="78"/>
+      <c r="C35" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="82"/>
-      <c r="I35" s="82"/>
-      <c r="J35" s="82"/>
-      <c r="K35" s="82"/>
-      <c r="L35" s="82"/>
-      <c r="M35" s="82"/>
-      <c r="N35" s="82"/>
-      <c r="O35" s="82"/>
-      <c r="P35" s="82"/>
-      <c r="Q35" s="82"/>
-      <c r="R35" s="82"/>
-      <c r="S35" s="82"/>
-      <c r="T35" s="80"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="78"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="78"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="78"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="78"/>
+      <c r="S35" s="78"/>
+      <c r="T35" s="76"/>
     </row>
     <row r="36" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="84" t="s">
+      <c r="A36" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="84"/>
-      <c r="H36" s="84"/>
-      <c r="I36" s="84"/>
-      <c r="J36" s="84"/>
-      <c r="K36" s="84"/>
-      <c r="L36" s="84"/>
-      <c r="M36" s="84"/>
-      <c r="N36" s="84"/>
-      <c r="O36" s="84"/>
-      <c r="P36" s="84"/>
-      <c r="Q36" s="84"/>
-      <c r="R36" s="84"/>
-      <c r="S36" s="84"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="80"/>
+      <c r="P36" s="80"/>
+      <c r="Q36" s="80"/>
+      <c r="R36" s="80"/>
+      <c r="S36" s="80"/>
       <c r="T36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3242,69 +3235,69 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="85"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="86"/>
-      <c r="M38" s="86"/>
-      <c r="N38" s="86"/>
-      <c r="O38" s="86"/>
-      <c r="P38" s="86"/>
-      <c r="Q38" s="86"/>
-      <c r="R38" s="86"/>
-      <c r="S38" s="87"/>
+      <c r="A38" s="81"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
+      <c r="R38" s="82"/>
+      <c r="S38" s="83"/>
       <c r="T38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="88"/>
-      <c r="B39" s="89"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="89"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="89"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="89"/>
-      <c r="M39" s="89"/>
-      <c r="N39" s="89"/>
-      <c r="O39" s="89"/>
-      <c r="P39" s="89"/>
-      <c r="Q39" s="89"/>
-      <c r="R39" s="89"/>
-      <c r="S39" s="90"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="85"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="85"/>
+      <c r="P39" s="85"/>
+      <c r="Q39" s="85"/>
+      <c r="R39" s="85"/>
+      <c r="S39" s="86"/>
       <c r="T39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="91"/>
-      <c r="B40" s="92"/>
-      <c r="C40" s="92"/>
-      <c r="D40" s="92"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="92"/>
-      <c r="G40" s="92"/>
-      <c r="H40" s="92"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="92"/>
-      <c r="K40" s="92"/>
-      <c r="L40" s="92"/>
-      <c r="M40" s="92"/>
-      <c r="N40" s="92"/>
-      <c r="O40" s="92"/>
-      <c r="P40" s="92"/>
-      <c r="Q40" s="92"/>
-      <c r="R40" s="92"/>
-      <c r="S40" s="93"/>
+      <c r="A40" s="87"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="88"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="88"/>
+      <c r="F40" s="88"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="88"/>
+      <c r="I40" s="88"/>
+      <c r="J40" s="88"/>
+      <c r="K40" s="88"/>
+      <c r="L40" s="88"/>
+      <c r="M40" s="88"/>
+      <c r="N40" s="88"/>
+      <c r="O40" s="88"/>
+      <c r="P40" s="88"/>
+      <c r="Q40" s="88"/>
+      <c r="R40" s="88"/>
+      <c r="S40" s="89"/>
       <c r="T40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3329,276 +3322,276 @@
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
     </row>
-    <row r="42" s="97" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="94" t="s">
+    <row r="42" s="93" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="94"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="95"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95"/>
-      <c r="I42" s="95"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="95"/>
-      <c r="L42" s="95"/>
-      <c r="M42" s="95"/>
-      <c r="N42" s="95"/>
-      <c r="O42" s="95"/>
-      <c r="P42" s="95"/>
-      <c r="Q42" s="95"/>
-      <c r="R42" s="95"/>
-      <c r="S42" s="95"/>
-      <c r="T42" s="96"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="91"/>
+      <c r="K42" s="91"/>
+      <c r="L42" s="91"/>
+      <c r="M42" s="91"/>
+      <c r="N42" s="91"/>
+      <c r="O42" s="91"/>
+      <c r="P42" s="91"/>
+      <c r="Q42" s="91"/>
+      <c r="R42" s="91"/>
+      <c r="S42" s="91"/>
+      <c r="T42" s="92"/>
     </row>
     <row r="43" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="83" t="s">
+      <c r="A43" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="98"/>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="95"/>
-      <c r="I43" s="95"/>
-      <c r="J43" s="95"/>
-      <c r="K43" s="95"/>
-      <c r="L43" s="95"/>
-      <c r="M43" s="95"/>
-      <c r="N43" s="95"/>
-      <c r="O43" s="95"/>
-      <c r="P43" s="95"/>
-      <c r="Q43" s="95"/>
-      <c r="R43" s="95"/>
-      <c r="S43" s="95"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="94"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
+      <c r="K43" s="91"/>
+      <c r="L43" s="91"/>
+      <c r="M43" s="91"/>
+      <c r="N43" s="91"/>
+      <c r="O43" s="91"/>
+      <c r="P43" s="91"/>
+      <c r="Q43" s="91"/>
+      <c r="R43" s="91"/>
+      <c r="S43" s="91"/>
       <c r="T43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="99" t="s">
+      <c r="A44" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="99"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="99"/>
-      <c r="E44" s="99"/>
-      <c r="F44" s="99"/>
-      <c r="G44" s="99"/>
-      <c r="H44" s="99"/>
-      <c r="I44" s="99"/>
-      <c r="J44" s="99"/>
-      <c r="K44" s="99"/>
-      <c r="L44" s="99"/>
-      <c r="M44" s="99"/>
-      <c r="N44" s="99"/>
-      <c r="O44" s="99"/>
-      <c r="P44" s="99"/>
-      <c r="Q44" s="99"/>
-      <c r="R44" s="99"/>
-      <c r="S44" s="99"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="95"/>
+      <c r="F44" s="95"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="95"/>
+      <c r="I44" s="95"/>
+      <c r="J44" s="95"/>
+      <c r="K44" s="95"/>
+      <c r="L44" s="95"/>
+      <c r="M44" s="95"/>
+      <c r="N44" s="95"/>
+      <c r="O44" s="95"/>
+      <c r="P44" s="95"/>
+      <c r="Q44" s="95"/>
+      <c r="R44" s="95"/>
+      <c r="S44" s="95"/>
       <c r="T44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="99"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="99"/>
-      <c r="D45" s="99"/>
-      <c r="E45" s="99"/>
-      <c r="F45" s="99"/>
-      <c r="G45" s="99"/>
-      <c r="H45" s="99"/>
-      <c r="I45" s="99"/>
-      <c r="J45" s="99"/>
-      <c r="K45" s="99"/>
-      <c r="L45" s="99"/>
-      <c r="M45" s="99"/>
-      <c r="N45" s="99"/>
-      <c r="O45" s="99"/>
-      <c r="P45" s="99"/>
-      <c r="Q45" s="99"/>
-      <c r="R45" s="99"/>
-      <c r="S45" s="99"/>
+      <c r="A45" s="95"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="95"/>
+      <c r="E45" s="95"/>
+      <c r="F45" s="95"/>
+      <c r="G45" s="95"/>
+      <c r="H45" s="95"/>
+      <c r="I45" s="95"/>
+      <c r="J45" s="95"/>
+      <c r="K45" s="95"/>
+      <c r="L45" s="95"/>
+      <c r="M45" s="95"/>
+      <c r="N45" s="95"/>
+      <c r="O45" s="95"/>
+      <c r="P45" s="95"/>
+      <c r="Q45" s="95"/>
+      <c r="R45" s="95"/>
+      <c r="S45" s="95"/>
       <c r="T45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="99"/>
-      <c r="B46" s="99"/>
-      <c r="C46" s="99"/>
-      <c r="D46" s="99"/>
-      <c r="E46" s="99"/>
-      <c r="F46" s="99"/>
-      <c r="G46" s="99"/>
-      <c r="H46" s="99"/>
-      <c r="I46" s="99"/>
-      <c r="J46" s="99"/>
-      <c r="K46" s="99"/>
-      <c r="L46" s="99"/>
-      <c r="M46" s="99"/>
-      <c r="N46" s="99"/>
-      <c r="O46" s="99"/>
-      <c r="P46" s="99"/>
-      <c r="Q46" s="99"/>
-      <c r="R46" s="99"/>
-      <c r="S46" s="99"/>
+      <c r="A46" s="95"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="95"/>
+      <c r="F46" s="95"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="95"/>
+      <c r="I46" s="95"/>
+      <c r="J46" s="95"/>
+      <c r="K46" s="95"/>
+      <c r="L46" s="95"/>
+      <c r="M46" s="95"/>
+      <c r="N46" s="95"/>
+      <c r="O46" s="95"/>
+      <c r="P46" s="95"/>
+      <c r="Q46" s="95"/>
+      <c r="R46" s="95"/>
+      <c r="S46" s="95"/>
       <c r="T46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="99"/>
-      <c r="B47" s="99"/>
-      <c r="C47" s="99"/>
-      <c r="D47" s="99"/>
-      <c r="E47" s="99"/>
-      <c r="F47" s="99"/>
-      <c r="G47" s="99"/>
-      <c r="H47" s="99"/>
-      <c r="I47" s="99"/>
-      <c r="J47" s="99"/>
-      <c r="K47" s="99"/>
-      <c r="L47" s="99"/>
-      <c r="M47" s="99"/>
-      <c r="N47" s="99"/>
-      <c r="O47" s="99"/>
-      <c r="P47" s="99"/>
-      <c r="Q47" s="99"/>
-      <c r="R47" s="99"/>
-      <c r="S47" s="99"/>
+      <c r="A47" s="95"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="95"/>
+      <c r="G47" s="95"/>
+      <c r="H47" s="95"/>
+      <c r="I47" s="95"/>
+      <c r="J47" s="95"/>
+      <c r="K47" s="95"/>
+      <c r="L47" s="95"/>
+      <c r="M47" s="95"/>
+      <c r="N47" s="95"/>
+      <c r="O47" s="95"/>
+      <c r="P47" s="95"/>
+      <c r="Q47" s="95"/>
+      <c r="R47" s="95"/>
+      <c r="S47" s="95"/>
       <c r="T47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="100"/>
-      <c r="B48" s="100"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="100"/>
-      <c r="E48" s="100"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="100"/>
-      <c r="J48" s="100"/>
-      <c r="K48" s="100"/>
-      <c r="L48" s="100"/>
-      <c r="M48" s="100"/>
-      <c r="N48" s="100"/>
-      <c r="O48" s="100"/>
-      <c r="P48" s="100"/>
-      <c r="Q48" s="100"/>
-      <c r="R48" s="100"/>
-      <c r="S48" s="100"/>
+      <c r="A48" s="96"/>
+      <c r="B48" s="96"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="96"/>
+      <c r="H48" s="96"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="96"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="96"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="96"/>
+      <c r="O48" s="96"/>
+      <c r="P48" s="96"/>
+      <c r="Q48" s="96"/>
+      <c r="R48" s="96"/>
+      <c r="S48" s="96"/>
       <c r="T48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="100"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
-      <c r="E49" s="100"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="100"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="100"/>
-      <c r="J49" s="100"/>
-      <c r="K49" s="100"/>
-      <c r="L49" s="100"/>
-      <c r="M49" s="100"/>
-      <c r="N49" s="100"/>
-      <c r="O49" s="100"/>
-      <c r="P49" s="100"/>
-      <c r="Q49" s="100"/>
-      <c r="R49" s="100"/>
-      <c r="S49" s="100"/>
+      <c r="A49" s="96"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="96"/>
+      <c r="H49" s="96"/>
+      <c r="I49" s="96"/>
+      <c r="J49" s="96"/>
+      <c r="K49" s="96"/>
+      <c r="L49" s="96"/>
+      <c r="M49" s="96"/>
+      <c r="N49" s="96"/>
+      <c r="O49" s="96"/>
+      <c r="P49" s="96"/>
+      <c r="Q49" s="96"/>
+      <c r="R49" s="96"/>
+      <c r="S49" s="96"/>
       <c r="T49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="100"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="100"/>
-      <c r="D50" s="100"/>
-      <c r="E50" s="100"/>
-      <c r="F50" s="100"/>
-      <c r="G50" s="100"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="100"/>
-      <c r="J50" s="100"/>
-      <c r="K50" s="100"/>
-      <c r="L50" s="100"/>
-      <c r="M50" s="100"/>
-      <c r="N50" s="100"/>
-      <c r="O50" s="100"/>
-      <c r="P50" s="100"/>
-      <c r="Q50" s="100"/>
-      <c r="R50" s="100"/>
-      <c r="S50" s="100"/>
+      <c r="A50" s="96"/>
+      <c r="B50" s="96"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="96"/>
+      <c r="K50" s="96"/>
+      <c r="L50" s="96"/>
+      <c r="M50" s="96"/>
+      <c r="N50" s="96"/>
+      <c r="O50" s="96"/>
+      <c r="P50" s="96"/>
+      <c r="Q50" s="96"/>
+      <c r="R50" s="96"/>
+      <c r="S50" s="96"/>
       <c r="T50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="100"/>
-      <c r="B51" s="100"/>
-      <c r="C51" s="100"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="100"/>
-      <c r="G51" s="100"/>
-      <c r="H51" s="100"/>
-      <c r="I51" s="100"/>
-      <c r="J51" s="100"/>
-      <c r="K51" s="100"/>
-      <c r="L51" s="100"/>
-      <c r="M51" s="100"/>
-      <c r="N51" s="100"/>
-      <c r="O51" s="100"/>
-      <c r="P51" s="100"/>
-      <c r="Q51" s="100"/>
-      <c r="R51" s="100"/>
-      <c r="S51" s="100"/>
+      <c r="A51" s="96"/>
+      <c r="B51" s="96"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="96"/>
+      <c r="E51" s="96"/>
+      <c r="F51" s="96"/>
+      <c r="G51" s="96"/>
+      <c r="H51" s="96"/>
+      <c r="I51" s="96"/>
+      <c r="J51" s="96"/>
+      <c r="K51" s="96"/>
+      <c r="L51" s="96"/>
+      <c r="M51" s="96"/>
+      <c r="N51" s="96"/>
+      <c r="O51" s="96"/>
+      <c r="P51" s="96"/>
+      <c r="Q51" s="96"/>
+      <c r="R51" s="96"/>
+      <c r="S51" s="96"/>
       <c r="T51" s="6"/>
     </row>
-    <row r="52" s="105" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="101"/>
-      <c r="B52" s="101"/>
-      <c r="C52" s="101"/>
-      <c r="D52" s="102" t="s">
+    <row r="52" s="101" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="97"/>
+      <c r="B52" s="97"/>
+      <c r="C52" s="97"/>
+      <c r="D52" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="102"/>
-      <c r="F52" s="102"/>
-      <c r="G52" s="102"/>
-      <c r="H52" s="102"/>
-      <c r="I52" s="102"/>
-      <c r="J52" s="102"/>
-      <c r="K52" s="103" t="s">
+      <c r="E52" s="98"/>
+      <c r="F52" s="98"/>
+      <c r="G52" s="98"/>
+      <c r="H52" s="98"/>
+      <c r="I52" s="98"/>
+      <c r="J52" s="98"/>
+      <c r="K52" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="L52" s="103"/>
-      <c r="M52" s="103"/>
-      <c r="N52" s="103"/>
-      <c r="O52" s="103"/>
-      <c r="P52" s="104"/>
-      <c r="Q52" s="104"/>
-      <c r="R52" s="101"/>
-      <c r="S52" s="101"/>
-      <c r="T52" s="101"/>
+      <c r="L52" s="99"/>
+      <c r="M52" s="99"/>
+      <c r="N52" s="99"/>
+      <c r="O52" s="99"/>
+      <c r="P52" s="100"/>
+      <c r="Q52" s="100"/>
+      <c r="R52" s="97"/>
+      <c r="S52" s="97"/>
+      <c r="T52" s="97"/>
     </row>
     <row r="53" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="106"/>
-      <c r="D53" s="107"/>
-      <c r="E53" s="108"/>
-      <c r="F53" s="108"/>
-      <c r="G53" s="108"/>
-      <c r="H53" s="108"/>
-      <c r="I53" s="108"/>
-      <c r="J53" s="109"/>
-      <c r="K53" s="110"/>
-      <c r="L53" s="110"/>
-      <c r="M53" s="110"/>
-      <c r="N53" s="110"/>
-      <c r="O53" s="111"/>
-      <c r="P53" s="112"/>
-      <c r="Q53" s="112"/>
+      <c r="C53" s="102"/>
+      <c r="D53" s="103"/>
+      <c r="E53" s="104"/>
+      <c r="F53" s="104"/>
+      <c r="G53" s="104"/>
+      <c r="H53" s="104"/>
+      <c r="I53" s="104"/>
+      <c r="J53" s="105"/>
+      <c r="K53" s="106"/>
+      <c r="L53" s="106"/>
+      <c r="M53" s="106"/>
+      <c r="N53" s="106"/>
+      <c r="O53" s="107"/>
+      <c r="P53" s="108"/>
+      <c r="Q53" s="108"/>
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="6"/>
@@ -3607,20 +3600,20 @@
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
-      <c r="D54" s="113"/>
-      <c r="E54" s="112"/>
-      <c r="F54" s="112"/>
-      <c r="G54" s="112"/>
-      <c r="H54" s="112"/>
-      <c r="I54" s="112"/>
-      <c r="J54" s="114"/>
-      <c r="K54" s="115"/>
-      <c r="L54" s="115"/>
-      <c r="M54" s="115"/>
-      <c r="N54" s="115"/>
-      <c r="O54" s="116"/>
-      <c r="P54" s="112"/>
-      <c r="Q54" s="117"/>
+      <c r="D54" s="109"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="108"/>
+      <c r="H54" s="108"/>
+      <c r="I54" s="108"/>
+      <c r="J54" s="110"/>
+      <c r="K54" s="111"/>
+      <c r="L54" s="111"/>
+      <c r="M54" s="111"/>
+      <c r="N54" s="111"/>
+      <c r="O54" s="112"/>
+      <c r="P54" s="108"/>
+      <c r="Q54" s="113"/>
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
       <c r="T54" s="6"/>
@@ -3628,21 +3621,21 @@
     <row r="55" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="113"/>
-      <c r="E55" s="112"/>
-      <c r="F55" s="112"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="112"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="114"/>
-      <c r="K55" s="115"/>
-      <c r="L55" s="115"/>
-      <c r="M55" s="115"/>
-      <c r="N55" s="115"/>
-      <c r="O55" s="116"/>
-      <c r="P55" s="119"/>
-      <c r="Q55" s="112"/>
+      <c r="C55" s="114"/>
+      <c r="D55" s="109"/>
+      <c r="E55" s="108"/>
+      <c r="F55" s="108"/>
+      <c r="G55" s="108"/>
+      <c r="H55" s="108"/>
+      <c r="I55" s="108"/>
+      <c r="J55" s="110"/>
+      <c r="K55" s="111"/>
+      <c r="L55" s="111"/>
+      <c r="M55" s="111"/>
+      <c r="N55" s="111"/>
+      <c r="O55" s="112"/>
+      <c r="P55" s="115"/>
+      <c r="Q55" s="108"/>
       <c r="R55" s="6"/>
       <c r="S55" s="6"/>
       <c r="T55" s="6"/>
@@ -3650,25 +3643,25 @@
     <row r="56" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="120" t="s">
+      <c r="C56" s="114"/>
+      <c r="D56" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="E56" s="120"/>
-      <c r="F56" s="120"/>
-      <c r="G56" s="121"/>
-      <c r="H56" s="121"/>
-      <c r="I56" s="121"/>
-      <c r="J56" s="121"/>
-      <c r="K56" s="120" t="s">
+      <c r="E56" s="116"/>
+      <c r="F56" s="116"/>
+      <c r="G56" s="117"/>
+      <c r="H56" s="117"/>
+      <c r="I56" s="117"/>
+      <c r="J56" s="117"/>
+      <c r="K56" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="L56" s="121"/>
-      <c r="M56" s="121"/>
-      <c r="N56" s="121"/>
-      <c r="O56" s="121"/>
-      <c r="P56" s="122"/>
-      <c r="Q56" s="112"/>
+      <c r="L56" s="118"/>
+      <c r="M56" s="118"/>
+      <c r="N56" s="118"/>
+      <c r="O56" s="118"/>
+      <c r="P56" s="119"/>
+      <c r="Q56" s="108"/>
       <c r="R56" s="6"/>
       <c r="S56" s="6"/>
       <c r="T56" s="6"/>
@@ -3676,23 +3669,23 @@
     <row r="57" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="123"/>
-      <c r="D57" s="124" t="s">
+      <c r="C57" s="120"/>
+      <c r="D57" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="125"/>
-      <c r="H57" s="125"/>
-      <c r="I57" s="125"/>
-      <c r="J57" s="125"/>
-      <c r="K57" s="126" t="s">
+      <c r="E57" s="121"/>
+      <c r="F57" s="121"/>
+      <c r="G57" s="122"/>
+      <c r="H57" s="122"/>
+      <c r="I57" s="122"/>
+      <c r="J57" s="122"/>
+      <c r="K57" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="L57" s="127"/>
-      <c r="M57" s="127"/>
-      <c r="N57" s="127"/>
-      <c r="O57" s="127"/>
+      <c r="L57" s="124"/>
+      <c r="M57" s="124"/>
+      <c r="N57" s="124"/>
+      <c r="O57" s="124"/>
       <c r="P57" s="6"/>
       <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
@@ -3702,19 +3695,19 @@
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="123"/>
-      <c r="D58" s="123"/>
-      <c r="E58" s="123"/>
-      <c r="F58" s="123"/>
-      <c r="G58" s="123"/>
-      <c r="H58" s="123"/>
-      <c r="I58" s="123"/>
-      <c r="J58" s="123"/>
-      <c r="K58" s="123"/>
-      <c r="L58" s="123"/>
-      <c r="M58" s="123"/>
-      <c r="N58" s="123"/>
-      <c r="O58" s="123"/>
+      <c r="C58" s="120"/>
+      <c r="D58" s="120"/>
+      <c r="E58" s="120"/>
+      <c r="F58" s="120"/>
+      <c r="G58" s="120"/>
+      <c r="H58" s="120"/>
+      <c r="I58" s="120"/>
+      <c r="J58" s="120"/>
+      <c r="K58" s="120"/>
+      <c r="L58" s="120"/>
+      <c r="M58" s="120"/>
+      <c r="N58" s="120"/>
+      <c r="O58" s="120"/>
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
       <c r="R58" s="6"/>
@@ -3722,7 +3715,7 @@
       <c r="T58" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="109">
+  <mergeCells count="111">
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="D1:P3"/>
     <mergeCell ref="Q1:R1"/>
@@ -3730,6 +3723,7 @@
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="A5:S5"/>
     <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:N7"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="D8:O8"/>
     <mergeCell ref="A9:C9"/>
@@ -3739,6 +3733,7 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D11:N11"/>
     <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:S11"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="N13:O13"/>
@@ -3885,79 +3880,79 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="128"/>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="129" t="s">
+      <c r="A1" s="125"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
-      <c r="P1" s="129"/>
-      <c r="Q1" s="130" t="s">
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="130"/>
-      <c r="S1" s="131"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="128"/>
       <c r="T1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="128"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="132" t="s">
+      <c r="A2" s="125"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="126"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="129" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="132"/>
-      <c r="S2" s="133" t="s">
+      <c r="R2" s="129"/>
+      <c r="S2" s="130" t="s">
         <v>4</v>
       </c>
       <c r="T2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="128"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="129"/>
-      <c r="O3" s="129"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="130" t="s">
+      <c r="A3" s="125"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="130"/>
-      <c r="S3" s="134" t="n">
+      <c r="R3" s="127"/>
+      <c r="S3" s="131" t="n">
         <v>45460</v>
       </c>
       <c r="T3" s="6"/>
@@ -3981,36 +3976,36 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="135"/>
+      <c r="S4" s="132"/>
       <c r="T4" s="6"/>
     </row>
     <row r="5" s="15" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="136" t="s">
+      <c r="A5" s="133" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="136"/>
-      <c r="O5" s="136"/>
-      <c r="P5" s="136"/>
-      <c r="Q5" s="136"/>
-      <c r="R5" s="136"/>
-      <c r="S5" s="136"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
+      <c r="N5" s="133"/>
+      <c r="O5" s="133"/>
+      <c r="P5" s="133"/>
+      <c r="Q5" s="133"/>
+      <c r="R5" s="133"/>
+      <c r="S5" s="133"/>
       <c r="T5" s="14"/>
     </row>
     <row r="6" s="15" customFormat="true" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -4031,95 +4026,95 @@
       <c r="T6" s="14"/>
     </row>
     <row r="7" s="15" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="137"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="138"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="138"/>
-      <c r="M7" s="138"/>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
-      <c r="P7" s="137" t="s">
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="135"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="135"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="137"/>
-      <c r="R7" s="139"/>
-      <c r="S7" s="139"/>
+      <c r="Q7" s="134"/>
+      <c r="R7" s="136"/>
+      <c r="S7" s="136"/>
       <c r="T7" s="14"/>
     </row>
     <row r="8" s="15" customFormat="true" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
       <c r="T8" s="14"/>
     </row>
     <row r="9" s="15" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="137" t="s">
+      <c r="A9" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
-      <c r="J9" s="140"/>
-      <c r="K9" s="140"/>
-      <c r="L9" s="140"/>
-      <c r="M9" s="140"/>
-      <c r="N9" s="140"/>
-      <c r="O9" s="140"/>
-      <c r="P9" s="137" t="s">
+      <c r="B9" s="134"/>
+      <c r="C9" s="134"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="137"/>
+      <c r="L9" s="137"/>
+      <c r="M9" s="137"/>
+      <c r="N9" s="137"/>
+      <c r="O9" s="137"/>
+      <c r="P9" s="134" t="s">
         <v>10</v>
       </c>
-      <c r="Q9" s="137"/>
-      <c r="R9" s="139"/>
-      <c r="S9" s="139"/>
+      <c r="Q9" s="134"/>
+      <c r="R9" s="136"/>
+      <c r="S9" s="136"/>
       <c r="T9" s="14"/>
     </row>
     <row r="10" s="15" customFormat="true" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
@@ -4127,36 +4122,36 @@
       <c r="T10" s="14"/>
     </row>
     <row r="11" s="15" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="137"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="140"/>
-      <c r="K11" s="140"/>
-      <c r="L11" s="140"/>
-      <c r="M11" s="140"/>
-      <c r="N11" s="140"/>
-      <c r="O11" s="140"/>
-      <c r="P11" s="137" t="s">
+      <c r="B11" s="134"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="137"/>
+      <c r="I11" s="137"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="137"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
+      <c r="O11" s="137"/>
+      <c r="P11" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" s="137"/>
-      <c r="R11" s="141" t="s">
+      <c r="Q11" s="134"/>
+      <c r="R11" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="S11" s="142"/>
+      <c r="S11" s="139"/>
       <c r="T11" s="14"/>
     </row>
     <row r="12" s="15" customFormat="true" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4174,45 +4169,45 @@
       <c r="T12" s="14"/>
     </row>
     <row r="13" s="15" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="143" t="s">
+      <c r="A13" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="143"/>
-      <c r="C13" s="143"/>
-      <c r="E13" s="144" t="s">
+      <c r="B13" s="140"/>
+      <c r="C13" s="140"/>
+      <c r="E13" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="144"/>
-      <c r="G13" s="144"/>
-      <c r="H13" s="145"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="144" t="s">
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="142"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="144"/>
-      <c r="L13" s="145"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="146" t="s">
+      <c r="K13" s="141"/>
+      <c r="L13" s="142"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="146"/>
-      <c r="P13" s="145"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
+      <c r="O13" s="143"/>
+      <c r="P13" s="142"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
       <c r="T13" s="14"/>
     </row>
     <row r="14" s="15" customFormat="true" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="14"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
@@ -4224,29 +4219,29 @@
       <c r="T14" s="14"/>
     </row>
     <row r="15" s="15" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="147" t="s">
+      <c r="E15" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="147"/>
-      <c r="G15" s="147"/>
-      <c r="H15" s="148"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="145"/>
       <c r="I15" s="14"/>
-      <c r="J15" s="147" t="s">
+      <c r="J15" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="147"/>
-      <c r="L15" s="149"/>
-      <c r="M15" s="149"/>
-      <c r="N15" s="149"/>
-      <c r="O15" s="149"/>
-      <c r="P15" s="149"/>
-      <c r="Q15" s="149"/>
-      <c r="R15" s="149"/>
-      <c r="S15" s="149"/>
+      <c r="K15" s="144"/>
+      <c r="L15" s="146"/>
+      <c r="M15" s="146"/>
+      <c r="N15" s="146"/>
+      <c r="O15" s="146"/>
+      <c r="P15" s="146"/>
+      <c r="Q15" s="146"/>
+      <c r="R15" s="146"/>
+      <c r="S15" s="146"/>
       <c r="T15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4272,32 +4267,32 @@
       <c r="T16" s="6"/>
     </row>
     <row r="17" s="15" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="136" t="s">
+      <c r="A17" s="133" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="136"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="136"/>
-      <c r="H17" s="136"/>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="136"/>
-      <c r="M17" s="136"/>
-      <c r="N17" s="136"/>
-      <c r="O17" s="136"/>
-      <c r="P17" s="136"/>
-      <c r="Q17" s="136"/>
-      <c r="R17" s="136"/>
-      <c r="S17" s="136"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
+      <c r="K17" s="133"/>
+      <c r="L17" s="133"/>
+      <c r="M17" s="133"/>
+      <c r="N17" s="133"/>
+      <c r="O17" s="133"/>
+      <c r="P17" s="133"/>
+      <c r="Q17" s="133"/>
+      <c r="R17" s="133"/>
+      <c r="S17" s="133"/>
       <c r="T17" s="14"/>
     </row>
     <row r="18" s="15" customFormat="true" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -4318,429 +4313,429 @@
       <c r="T18" s="14"/>
     </row>
     <row r="19" s="15" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="147" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="150"/>
-      <c r="C19" s="150"/>
-      <c r="D19" s="150"/>
-      <c r="E19" s="150"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="150"/>
-      <c r="H19" s="150"/>
-      <c r="I19" s="150"/>
-      <c r="J19" s="150"/>
-      <c r="K19" s="150"/>
-      <c r="L19" s="150"/>
-      <c r="M19" s="150"/>
-      <c r="N19" s="150"/>
-      <c r="O19" s="150"/>
-      <c r="P19" s="150"/>
-      <c r="Q19" s="150"/>
-      <c r="R19" s="150"/>
-      <c r="S19" s="150"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="147"/>
+      <c r="D19" s="147"/>
+      <c r="E19" s="147"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="147"/>
+      <c r="H19" s="147"/>
+      <c r="I19" s="147"/>
+      <c r="J19" s="147"/>
+      <c r="K19" s="147"/>
+      <c r="L19" s="147"/>
+      <c r="M19" s="147"/>
+      <c r="N19" s="147"/>
+      <c r="O19" s="147"/>
+      <c r="P19" s="147"/>
+      <c r="Q19" s="147"/>
+      <c r="R19" s="147"/>
+      <c r="S19" s="147"/>
       <c r="T19" s="14"/>
     </row>
     <row r="20" s="15" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="151" t="s">
+      <c r="A20" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="151" t="s">
+      <c r="B20" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="151"/>
-      <c r="D20" s="151" t="s">
+      <c r="C20" s="148"/>
+      <c r="D20" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151" t="s">
+      <c r="E20" s="148"/>
+      <c r="F20" s="148"/>
+      <c r="G20" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="151" t="s">
+      <c r="H20" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="151"/>
-      <c r="J20" s="151"/>
-      <c r="K20" s="151" t="s">
+      <c r="I20" s="148"/>
+      <c r="J20" s="148"/>
+      <c r="K20" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="L20" s="151"/>
-      <c r="M20" s="151" t="s">
+      <c r="L20" s="148"/>
+      <c r="M20" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="N20" s="151"/>
-      <c r="O20" s="151" t="s">
+      <c r="N20" s="148"/>
+      <c r="O20" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="P20" s="151"/>
-      <c r="Q20" s="151" t="s">
+      <c r="P20" s="148"/>
+      <c r="Q20" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="R20" s="151"/>
-      <c r="S20" s="151"/>
+      <c r="R20" s="148"/>
+      <c r="S20" s="148"/>
       <c r="T20" s="14"/>
     </row>
     <row r="21" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="149"/>
-      <c r="B21" s="149"/>
-      <c r="C21" s="149"/>
-      <c r="D21" s="149"/>
-      <c r="E21" s="149"/>
-      <c r="F21" s="149"/>
-      <c r="G21" s="152"/>
-      <c r="H21" s="153"/>
-      <c r="I21" s="153"/>
-      <c r="J21" s="153"/>
-      <c r="K21" s="154"/>
-      <c r="L21" s="154"/>
-      <c r="M21" s="155"/>
-      <c r="N21" s="155"/>
-      <c r="O21" s="155"/>
-      <c r="P21" s="155"/>
-      <c r="Q21" s="156"/>
-      <c r="R21" s="156"/>
-      <c r="S21" s="156"/>
+      <c r="A21" s="146"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="146"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="146"/>
+      <c r="F21" s="146"/>
+      <c r="G21" s="149"/>
+      <c r="H21" s="150"/>
+      <c r="I21" s="150"/>
+      <c r="J21" s="150"/>
+      <c r="K21" s="151"/>
+      <c r="L21" s="151"/>
+      <c r="M21" s="152"/>
+      <c r="N21" s="152"/>
+      <c r="O21" s="152"/>
+      <c r="P21" s="152"/>
+      <c r="Q21" s="153"/>
+      <c r="R21" s="153"/>
+      <c r="S21" s="153"/>
       <c r="T21" s="14"/>
     </row>
     <row r="22" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="149"/>
-      <c r="B22" s="149"/>
-      <c r="C22" s="149"/>
-      <c r="D22" s="149"/>
-      <c r="E22" s="149"/>
-      <c r="F22" s="149"/>
-      <c r="G22" s="152"/>
-      <c r="H22" s="153"/>
-      <c r="I22" s="153"/>
-      <c r="J22" s="153"/>
-      <c r="K22" s="154"/>
-      <c r="L22" s="154"/>
-      <c r="M22" s="155"/>
-      <c r="N22" s="155"/>
-      <c r="O22" s="155"/>
-      <c r="P22" s="155"/>
-      <c r="Q22" s="156"/>
-      <c r="R22" s="156"/>
-      <c r="S22" s="156"/>
+      <c r="A22" s="146"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="149"/>
+      <c r="H22" s="150"/>
+      <c r="I22" s="150"/>
+      <c r="J22" s="150"/>
+      <c r="K22" s="151"/>
+      <c r="L22" s="151"/>
+      <c r="M22" s="152"/>
+      <c r="N22" s="152"/>
+      <c r="O22" s="152"/>
+      <c r="P22" s="152"/>
+      <c r="Q22" s="153"/>
+      <c r="R22" s="153"/>
+      <c r="S22" s="153"/>
       <c r="T22" s="14"/>
     </row>
     <row r="23" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="149"/>
-      <c r="B23" s="149"/>
-      <c r="C23" s="149"/>
-      <c r="D23" s="149"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="149"/>
-      <c r="G23" s="152"/>
-      <c r="H23" s="153"/>
-      <c r="I23" s="153"/>
-      <c r="J23" s="153"/>
-      <c r="K23" s="154"/>
-      <c r="L23" s="154"/>
-      <c r="M23" s="155"/>
-      <c r="N23" s="155"/>
-      <c r="O23" s="155"/>
-      <c r="P23" s="155"/>
-      <c r="Q23" s="156"/>
-      <c r="R23" s="156"/>
-      <c r="S23" s="156"/>
+      <c r="A23" s="146"/>
+      <c r="B23" s="146"/>
+      <c r="C23" s="146"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="149"/>
+      <c r="H23" s="150"/>
+      <c r="I23" s="150"/>
+      <c r="J23" s="150"/>
+      <c r="K23" s="151"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="152"/>
+      <c r="N23" s="152"/>
+      <c r="O23" s="152"/>
+      <c r="P23" s="152"/>
+      <c r="Q23" s="153"/>
+      <c r="R23" s="153"/>
+      <c r="S23" s="153"/>
       <c r="T23" s="14"/>
     </row>
     <row r="24" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="149"/>
-      <c r="B24" s="149"/>
-      <c r="C24" s="149"/>
-      <c r="D24" s="149"/>
-      <c r="E24" s="149"/>
-      <c r="F24" s="149"/>
-      <c r="G24" s="152"/>
-      <c r="H24" s="153"/>
-      <c r="I24" s="153"/>
-      <c r="J24" s="153"/>
-      <c r="K24" s="154"/>
-      <c r="L24" s="154"/>
-      <c r="M24" s="155"/>
-      <c r="N24" s="155"/>
-      <c r="O24" s="155"/>
-      <c r="P24" s="155"/>
-      <c r="Q24" s="156"/>
-      <c r="R24" s="156"/>
-      <c r="S24" s="156"/>
+      <c r="A24" s="146"/>
+      <c r="B24" s="146"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="146"/>
+      <c r="E24" s="146"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="149"/>
+      <c r="H24" s="150"/>
+      <c r="I24" s="150"/>
+      <c r="J24" s="150"/>
+      <c r="K24" s="151"/>
+      <c r="L24" s="151"/>
+      <c r="M24" s="152"/>
+      <c r="N24" s="152"/>
+      <c r="O24" s="152"/>
+      <c r="P24" s="152"/>
+      <c r="Q24" s="153"/>
+      <c r="R24" s="153"/>
+      <c r="S24" s="153"/>
       <c r="T24" s="14"/>
     </row>
     <row r="25" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="149"/>
-      <c r="B25" s="149"/>
-      <c r="C25" s="149"/>
-      <c r="D25" s="149"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="149"/>
-      <c r="G25" s="152"/>
-      <c r="H25" s="153"/>
-      <c r="I25" s="153"/>
-      <c r="J25" s="153"/>
-      <c r="K25" s="154"/>
-      <c r="L25" s="154"/>
-      <c r="M25" s="155"/>
-      <c r="N25" s="155"/>
-      <c r="O25" s="155"/>
-      <c r="P25" s="155"/>
-      <c r="Q25" s="156"/>
-      <c r="R25" s="156"/>
-      <c r="S25" s="156"/>
+      <c r="A25" s="146"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="146"/>
+      <c r="D25" s="146"/>
+      <c r="E25" s="146"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="149"/>
+      <c r="H25" s="150"/>
+      <c r="I25" s="150"/>
+      <c r="J25" s="150"/>
+      <c r="K25" s="151"/>
+      <c r="L25" s="151"/>
+      <c r="M25" s="152"/>
+      <c r="N25" s="152"/>
+      <c r="O25" s="152"/>
+      <c r="P25" s="152"/>
+      <c r="Q25" s="153"/>
+      <c r="R25" s="153"/>
+      <c r="S25" s="153"/>
       <c r="T25" s="14"/>
     </row>
     <row r="26" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="149"/>
-      <c r="B26" s="149"/>
-      <c r="C26" s="149"/>
-      <c r="D26" s="149"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="149"/>
-      <c r="G26" s="152"/>
-      <c r="H26" s="153"/>
-      <c r="I26" s="153"/>
-      <c r="J26" s="153"/>
-      <c r="K26" s="154"/>
-      <c r="L26" s="154"/>
-      <c r="M26" s="155"/>
-      <c r="N26" s="155"/>
-      <c r="O26" s="155"/>
-      <c r="P26" s="155"/>
-      <c r="Q26" s="156"/>
-      <c r="R26" s="156"/>
-      <c r="S26" s="156"/>
+      <c r="A26" s="146"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="149"/>
+      <c r="H26" s="150"/>
+      <c r="I26" s="150"/>
+      <c r="J26" s="150"/>
+      <c r="K26" s="151"/>
+      <c r="L26" s="151"/>
+      <c r="M26" s="152"/>
+      <c r="N26" s="152"/>
+      <c r="O26" s="152"/>
+      <c r="P26" s="152"/>
+      <c r="Q26" s="153"/>
+      <c r="R26" s="153"/>
+      <c r="S26" s="153"/>
       <c r="T26" s="14"/>
     </row>
     <row r="27" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="149"/>
-      <c r="B27" s="149"/>
-      <c r="C27" s="149"/>
-      <c r="D27" s="149"/>
-      <c r="E27" s="149"/>
-      <c r="F27" s="149"/>
-      <c r="G27" s="152"/>
-      <c r="H27" s="153"/>
-      <c r="I27" s="153"/>
-      <c r="J27" s="153"/>
-      <c r="K27" s="154"/>
-      <c r="L27" s="154"/>
-      <c r="M27" s="155"/>
-      <c r="N27" s="155"/>
-      <c r="O27" s="155"/>
-      <c r="P27" s="155"/>
-      <c r="Q27" s="156"/>
-      <c r="R27" s="156"/>
-      <c r="S27" s="156"/>
+      <c r="A27" s="146"/>
+      <c r="B27" s="146"/>
+      <c r="C27" s="146"/>
+      <c r="D27" s="146"/>
+      <c r="E27" s="146"/>
+      <c r="F27" s="146"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="150"/>
+      <c r="I27" s="150"/>
+      <c r="J27" s="150"/>
+      <c r="K27" s="151"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="152"/>
+      <c r="N27" s="152"/>
+      <c r="O27" s="152"/>
+      <c r="P27" s="152"/>
+      <c r="Q27" s="153"/>
+      <c r="R27" s="153"/>
+      <c r="S27" s="153"/>
       <c r="T27" s="14"/>
     </row>
     <row r="28" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="149"/>
-      <c r="B28" s="149"/>
-      <c r="C28" s="149"/>
-      <c r="D28" s="149"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
-      <c r="G28" s="152"/>
-      <c r="H28" s="153"/>
-      <c r="I28" s="153"/>
-      <c r="J28" s="153"/>
-      <c r="K28" s="154"/>
-      <c r="L28" s="154"/>
-      <c r="M28" s="155"/>
-      <c r="N28" s="155"/>
-      <c r="O28" s="155"/>
-      <c r="P28" s="155"/>
-      <c r="Q28" s="156"/>
-      <c r="R28" s="156"/>
-      <c r="S28" s="156"/>
+      <c r="A28" s="146"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="149"/>
+      <c r="H28" s="150"/>
+      <c r="I28" s="150"/>
+      <c r="J28" s="150"/>
+      <c r="K28" s="151"/>
+      <c r="L28" s="151"/>
+      <c r="M28" s="152"/>
+      <c r="N28" s="152"/>
+      <c r="O28" s="152"/>
+      <c r="P28" s="152"/>
+      <c r="Q28" s="153"/>
+      <c r="R28" s="153"/>
+      <c r="S28" s="153"/>
       <c r="T28" s="14"/>
     </row>
     <row r="29" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="149"/>
-      <c r="B29" s="149"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
-      <c r="G29" s="152"/>
-      <c r="H29" s="153"/>
-      <c r="I29" s="153"/>
-      <c r="J29" s="153"/>
-      <c r="K29" s="154"/>
-      <c r="L29" s="154"/>
-      <c r="M29" s="155"/>
-      <c r="N29" s="155"/>
-      <c r="O29" s="155"/>
-      <c r="P29" s="155"/>
-      <c r="Q29" s="156"/>
-      <c r="R29" s="156"/>
-      <c r="S29" s="156"/>
+      <c r="A29" s="146"/>
+      <c r="B29" s="146"/>
+      <c r="C29" s="146"/>
+      <c r="D29" s="146"/>
+      <c r="E29" s="146"/>
+      <c r="F29" s="146"/>
+      <c r="G29" s="149"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="151"/>
+      <c r="L29" s="151"/>
+      <c r="M29" s="152"/>
+      <c r="N29" s="152"/>
+      <c r="O29" s="152"/>
+      <c r="P29" s="152"/>
+      <c r="Q29" s="153"/>
+      <c r="R29" s="153"/>
+      <c r="S29" s="153"/>
       <c r="T29" s="14"/>
     </row>
     <row r="30" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="149"/>
-      <c r="B30" s="149"/>
-      <c r="C30" s="149"/>
-      <c r="D30" s="149"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="149"/>
-      <c r="G30" s="152"/>
-      <c r="H30" s="153"/>
-      <c r="I30" s="153"/>
-      <c r="J30" s="153"/>
-      <c r="K30" s="154"/>
-      <c r="L30" s="154"/>
-      <c r="M30" s="155"/>
-      <c r="N30" s="155"/>
-      <c r="O30" s="155"/>
-      <c r="P30" s="155"/>
-      <c r="Q30" s="156"/>
-      <c r="R30" s="156"/>
-      <c r="S30" s="156"/>
+      <c r="A30" s="146"/>
+      <c r="B30" s="146"/>
+      <c r="C30" s="146"/>
+      <c r="D30" s="146"/>
+      <c r="E30" s="146"/>
+      <c r="F30" s="146"/>
+      <c r="G30" s="149"/>
+      <c r="H30" s="150"/>
+      <c r="I30" s="150"/>
+      <c r="J30" s="150"/>
+      <c r="K30" s="151"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="152"/>
+      <c r="N30" s="152"/>
+      <c r="O30" s="152"/>
+      <c r="P30" s="152"/>
+      <c r="Q30" s="153"/>
+      <c r="R30" s="153"/>
+      <c r="S30" s="153"/>
       <c r="T30" s="14"/>
     </row>
     <row r="31" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="149"/>
-      <c r="B31" s="149"/>
-      <c r="C31" s="149"/>
-      <c r="D31" s="149"/>
-      <c r="E31" s="149"/>
-      <c r="F31" s="149"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="153"/>
-      <c r="I31" s="153"/>
-      <c r="J31" s="153"/>
-      <c r="K31" s="154"/>
-      <c r="L31" s="154"/>
-      <c r="M31" s="155"/>
-      <c r="N31" s="155"/>
-      <c r="O31" s="155"/>
-      <c r="P31" s="155"/>
-      <c r="Q31" s="156"/>
-      <c r="R31" s="156"/>
-      <c r="S31" s="156"/>
+      <c r="A31" s="146"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="149"/>
+      <c r="H31" s="150"/>
+      <c r="I31" s="150"/>
+      <c r="J31" s="150"/>
+      <c r="K31" s="151"/>
+      <c r="L31" s="151"/>
+      <c r="M31" s="152"/>
+      <c r="N31" s="152"/>
+      <c r="O31" s="152"/>
+      <c r="P31" s="152"/>
+      <c r="Q31" s="153"/>
+      <c r="R31" s="153"/>
+      <c r="S31" s="153"/>
       <c r="T31" s="14"/>
     </row>
     <row r="32" s="15" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="149"/>
-      <c r="B32" s="149"/>
-      <c r="C32" s="149"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="152"/>
-      <c r="H32" s="153"/>
-      <c r="I32" s="153"/>
-      <c r="J32" s="153"/>
-      <c r="K32" s="154"/>
-      <c r="L32" s="154"/>
-      <c r="M32" s="155"/>
-      <c r="N32" s="155"/>
-      <c r="O32" s="155"/>
-      <c r="P32" s="155"/>
-      <c r="Q32" s="156"/>
-      <c r="R32" s="156"/>
-      <c r="S32" s="156"/>
+      <c r="A32" s="146"/>
+      <c r="B32" s="146"/>
+      <c r="C32" s="146"/>
+      <c r="D32" s="146"/>
+      <c r="E32" s="146"/>
+      <c r="F32" s="146"/>
+      <c r="G32" s="149"/>
+      <c r="H32" s="150"/>
+      <c r="I32" s="150"/>
+      <c r="J32" s="150"/>
+      <c r="K32" s="151"/>
+      <c r="L32" s="151"/>
+      <c r="M32" s="152"/>
+      <c r="N32" s="152"/>
+      <c r="O32" s="152"/>
+      <c r="P32" s="152"/>
+      <c r="Q32" s="153"/>
+      <c r="R32" s="153"/>
+      <c r="S32" s="153"/>
       <c r="T32" s="14"/>
     </row>
-    <row r="33" s="81" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="157" t="s">
+    <row r="33" s="77" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="154" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="158"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="80"/>
-      <c r="G33" s="80"/>
-      <c r="H33" s="80"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="80"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="80"/>
-      <c r="N33" s="80"/>
-      <c r="O33" s="159"/>
-      <c r="P33" s="160"/>
-      <c r="Q33" s="161"/>
-      <c r="R33" s="162"/>
-      <c r="S33" s="163"/>
-      <c r="T33" s="80"/>
-    </row>
-    <row r="34" s="81" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="158" t="s">
+      <c r="B33" s="155"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="76"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="76"/>
+      <c r="L33" s="76"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="76"/>
+      <c r="O33" s="156"/>
+      <c r="P33" s="157"/>
+      <c r="Q33" s="158"/>
+      <c r="R33" s="159"/>
+      <c r="S33" s="160"/>
+      <c r="T33" s="76"/>
+    </row>
+    <row r="34" s="77" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="158"/>
-      <c r="C34" s="164" t="s">
+      <c r="B34" s="155"/>
+      <c r="C34" s="161" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="164"/>
-      <c r="E34" s="164"/>
-      <c r="F34" s="164"/>
-      <c r="G34" s="164"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="80"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="80"/>
-      <c r="M34" s="80"/>
-      <c r="N34" s="80"/>
-      <c r="O34" s="80"/>
-      <c r="P34" s="80"/>
-      <c r="Q34" s="80"/>
-      <c r="R34" s="80"/>
-      <c r="S34" s="80"/>
-      <c r="T34" s="80"/>
-    </row>
-    <row r="35" s="81" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="165" t="s">
+      <c r="D34" s="161"/>
+      <c r="E34" s="161"/>
+      <c r="F34" s="161"/>
+      <c r="G34" s="161"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="76"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="76"/>
+      <c r="S34" s="76"/>
+      <c r="T34" s="76"/>
+    </row>
+    <row r="35" s="77" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="162" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="165"/>
-      <c r="C35" s="165"/>
-      <c r="D35" s="165"/>
-      <c r="E35" s="165"/>
-      <c r="F35" s="165"/>
-      <c r="G35" s="165"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="165"/>
-      <c r="J35" s="165"/>
-      <c r="K35" s="165"/>
-      <c r="L35" s="165"/>
-      <c r="M35" s="165"/>
-      <c r="N35" s="165"/>
-      <c r="O35" s="165"/>
-      <c r="P35" s="165"/>
-      <c r="Q35" s="165"/>
-      <c r="R35" s="165"/>
-      <c r="S35" s="165"/>
-      <c r="T35" s="80"/>
+      <c r="B35" s="162"/>
+      <c r="C35" s="162"/>
+      <c r="D35" s="162"/>
+      <c r="E35" s="162"/>
+      <c r="F35" s="162"/>
+      <c r="G35" s="162"/>
+      <c r="H35" s="162"/>
+      <c r="I35" s="162"/>
+      <c r="J35" s="162"/>
+      <c r="K35" s="162"/>
+      <c r="L35" s="162"/>
+      <c r="M35" s="162"/>
+      <c r="N35" s="162"/>
+      <c r="O35" s="162"/>
+      <c r="P35" s="162"/>
+      <c r="Q35" s="162"/>
+      <c r="R35" s="162"/>
+      <c r="S35" s="162"/>
+      <c r="T35" s="76"/>
     </row>
     <row r="36" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="136" t="s">
+      <c r="A36" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="136"/>
-      <c r="C36" s="136"/>
-      <c r="D36" s="136"/>
-      <c r="E36" s="136"/>
-      <c r="F36" s="136"/>
-      <c r="G36" s="136"/>
-      <c r="H36" s="136"/>
-      <c r="I36" s="136"/>
-      <c r="J36" s="136"/>
-      <c r="K36" s="136"/>
-      <c r="L36" s="136"/>
-      <c r="M36" s="136"/>
-      <c r="N36" s="136"/>
-      <c r="O36" s="136"/>
-      <c r="P36" s="136"/>
-      <c r="Q36" s="136"/>
-      <c r="R36" s="136"/>
-      <c r="S36" s="136"/>
+      <c r="B36" s="133"/>
+      <c r="C36" s="133"/>
+      <c r="D36" s="133"/>
+      <c r="E36" s="133"/>
+      <c r="F36" s="133"/>
+      <c r="G36" s="133"/>
+      <c r="H36" s="133"/>
+      <c r="I36" s="133"/>
+      <c r="J36" s="133"/>
+      <c r="K36" s="133"/>
+      <c r="L36" s="133"/>
+      <c r="M36" s="133"/>
+      <c r="N36" s="133"/>
+      <c r="O36" s="133"/>
+      <c r="P36" s="133"/>
+      <c r="Q36" s="133"/>
+      <c r="R36" s="133"/>
+      <c r="S36" s="133"/>
       <c r="T36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4766,69 +4761,69 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="153"/>
-      <c r="B38" s="153"/>
-      <c r="C38" s="153"/>
-      <c r="D38" s="153"/>
-      <c r="E38" s="153"/>
-      <c r="F38" s="153"/>
-      <c r="G38" s="153"/>
-      <c r="H38" s="153"/>
-      <c r="I38" s="153"/>
-      <c r="J38" s="153"/>
-      <c r="K38" s="153"/>
-      <c r="L38" s="153"/>
-      <c r="M38" s="153"/>
-      <c r="N38" s="153"/>
-      <c r="O38" s="153"/>
-      <c r="P38" s="153"/>
-      <c r="Q38" s="153"/>
-      <c r="R38" s="153"/>
-      <c r="S38" s="153"/>
+      <c r="A38" s="150"/>
+      <c r="B38" s="150"/>
+      <c r="C38" s="150"/>
+      <c r="D38" s="150"/>
+      <c r="E38" s="150"/>
+      <c r="F38" s="150"/>
+      <c r="G38" s="150"/>
+      <c r="H38" s="150"/>
+      <c r="I38" s="150"/>
+      <c r="J38" s="150"/>
+      <c r="K38" s="150"/>
+      <c r="L38" s="150"/>
+      <c r="M38" s="150"/>
+      <c r="N38" s="150"/>
+      <c r="O38" s="150"/>
+      <c r="P38" s="150"/>
+      <c r="Q38" s="150"/>
+      <c r="R38" s="150"/>
+      <c r="S38" s="150"/>
       <c r="T38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="153"/>
-      <c r="B39" s="153"/>
-      <c r="C39" s="153"/>
-      <c r="D39" s="153"/>
-      <c r="E39" s="153"/>
-      <c r="F39" s="153"/>
-      <c r="G39" s="153"/>
-      <c r="H39" s="153"/>
-      <c r="I39" s="153"/>
-      <c r="J39" s="153"/>
-      <c r="K39" s="153"/>
-      <c r="L39" s="153"/>
-      <c r="M39" s="153"/>
-      <c r="N39" s="153"/>
-      <c r="O39" s="153"/>
-      <c r="P39" s="153"/>
-      <c r="Q39" s="153"/>
-      <c r="R39" s="153"/>
-      <c r="S39" s="153"/>
+      <c r="A39" s="150"/>
+      <c r="B39" s="150"/>
+      <c r="C39" s="150"/>
+      <c r="D39" s="150"/>
+      <c r="E39" s="150"/>
+      <c r="F39" s="150"/>
+      <c r="G39" s="150"/>
+      <c r="H39" s="150"/>
+      <c r="I39" s="150"/>
+      <c r="J39" s="150"/>
+      <c r="K39" s="150"/>
+      <c r="L39" s="150"/>
+      <c r="M39" s="150"/>
+      <c r="N39" s="150"/>
+      <c r="O39" s="150"/>
+      <c r="P39" s="150"/>
+      <c r="Q39" s="150"/>
+      <c r="R39" s="150"/>
+      <c r="S39" s="150"/>
       <c r="T39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="153"/>
-      <c r="B40" s="153"/>
-      <c r="C40" s="153"/>
-      <c r="D40" s="153"/>
-      <c r="E40" s="153"/>
-      <c r="F40" s="153"/>
-      <c r="G40" s="153"/>
-      <c r="H40" s="153"/>
-      <c r="I40" s="153"/>
-      <c r="J40" s="153"/>
-      <c r="K40" s="153"/>
-      <c r="L40" s="153"/>
-      <c r="M40" s="153"/>
-      <c r="N40" s="153"/>
-      <c r="O40" s="153"/>
-      <c r="P40" s="153"/>
-      <c r="Q40" s="153"/>
-      <c r="R40" s="153"/>
-      <c r="S40" s="153"/>
+      <c r="A40" s="150"/>
+      <c r="B40" s="150"/>
+      <c r="C40" s="150"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="150"/>
+      <c r="F40" s="150"/>
+      <c r="G40" s="150"/>
+      <c r="H40" s="150"/>
+      <c r="I40" s="150"/>
+      <c r="J40" s="150"/>
+      <c r="K40" s="150"/>
+      <c r="L40" s="150"/>
+      <c r="M40" s="150"/>
+      <c r="N40" s="150"/>
+      <c r="O40" s="150"/>
+      <c r="P40" s="150"/>
+      <c r="Q40" s="150"/>
+      <c r="R40" s="150"/>
+      <c r="S40" s="150"/>
       <c r="T40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4854,10 +4849,10 @@
       <c r="T41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="101" t="s">
+      <c r="A42" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="166"/>
+      <c r="B42" s="163"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -4878,10 +4873,10 @@
       <c r="T42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="167" t="s">
+      <c r="A43" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="168"/>
+      <c r="B43" s="165"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -4902,231 +4897,231 @@
       <c r="T43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="169" t="s">
+      <c r="A44" s="166" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="169"/>
-      <c r="C44" s="169"/>
-      <c r="D44" s="169"/>
-      <c r="E44" s="169"/>
-      <c r="F44" s="169"/>
-      <c r="G44" s="169"/>
-      <c r="H44" s="169"/>
-      <c r="I44" s="169"/>
-      <c r="J44" s="169"/>
-      <c r="K44" s="169"/>
-      <c r="L44" s="169"/>
-      <c r="M44" s="169"/>
-      <c r="N44" s="169"/>
-      <c r="O44" s="169"/>
-      <c r="P44" s="169"/>
-      <c r="Q44" s="169"/>
-      <c r="R44" s="169"/>
-      <c r="S44" s="169"/>
+      <c r="B44" s="166"/>
+      <c r="C44" s="166"/>
+      <c r="D44" s="166"/>
+      <c r="E44" s="166"/>
+      <c r="F44" s="166"/>
+      <c r="G44" s="166"/>
+      <c r="H44" s="166"/>
+      <c r="I44" s="166"/>
+      <c r="J44" s="166"/>
+      <c r="K44" s="166"/>
+      <c r="L44" s="166"/>
+      <c r="M44" s="166"/>
+      <c r="N44" s="166"/>
+      <c r="O44" s="166"/>
+      <c r="P44" s="166"/>
+      <c r="Q44" s="166"/>
+      <c r="R44" s="166"/>
+      <c r="S44" s="166"/>
       <c r="T44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="169"/>
-      <c r="B45" s="169"/>
-      <c r="C45" s="169"/>
-      <c r="D45" s="169"/>
-      <c r="E45" s="169"/>
-      <c r="F45" s="169"/>
-      <c r="G45" s="169"/>
-      <c r="H45" s="169"/>
-      <c r="I45" s="169"/>
-      <c r="J45" s="169"/>
-      <c r="K45" s="169"/>
-      <c r="L45" s="169"/>
-      <c r="M45" s="169"/>
-      <c r="N45" s="169"/>
-      <c r="O45" s="169"/>
-      <c r="P45" s="169"/>
-      <c r="Q45" s="169"/>
-      <c r="R45" s="169"/>
-      <c r="S45" s="169"/>
+      <c r="A45" s="166"/>
+      <c r="B45" s="166"/>
+      <c r="C45" s="166"/>
+      <c r="D45" s="166"/>
+      <c r="E45" s="166"/>
+      <c r="F45" s="166"/>
+      <c r="G45" s="166"/>
+      <c r="H45" s="166"/>
+      <c r="I45" s="166"/>
+      <c r="J45" s="166"/>
+      <c r="K45" s="166"/>
+      <c r="L45" s="166"/>
+      <c r="M45" s="166"/>
+      <c r="N45" s="166"/>
+      <c r="O45" s="166"/>
+      <c r="P45" s="166"/>
+      <c r="Q45" s="166"/>
+      <c r="R45" s="166"/>
+      <c r="S45" s="166"/>
       <c r="T45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="169"/>
-      <c r="B46" s="169"/>
-      <c r="C46" s="169"/>
-      <c r="D46" s="169"/>
-      <c r="E46" s="169"/>
-      <c r="F46" s="169"/>
-      <c r="G46" s="169"/>
-      <c r="H46" s="169"/>
-      <c r="I46" s="169"/>
-      <c r="J46" s="169"/>
-      <c r="K46" s="169"/>
-      <c r="L46" s="169"/>
-      <c r="M46" s="169"/>
-      <c r="N46" s="169"/>
-      <c r="O46" s="169"/>
-      <c r="P46" s="169"/>
-      <c r="Q46" s="169"/>
-      <c r="R46" s="169"/>
-      <c r="S46" s="169"/>
+      <c r="A46" s="166"/>
+      <c r="B46" s="166"/>
+      <c r="C46" s="166"/>
+      <c r="D46" s="166"/>
+      <c r="E46" s="166"/>
+      <c r="F46" s="166"/>
+      <c r="G46" s="166"/>
+      <c r="H46" s="166"/>
+      <c r="I46" s="166"/>
+      <c r="J46" s="166"/>
+      <c r="K46" s="166"/>
+      <c r="L46" s="166"/>
+      <c r="M46" s="166"/>
+      <c r="N46" s="166"/>
+      <c r="O46" s="166"/>
+      <c r="P46" s="166"/>
+      <c r="Q46" s="166"/>
+      <c r="R46" s="166"/>
+      <c r="S46" s="166"/>
       <c r="T46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="169"/>
-      <c r="B47" s="169"/>
-      <c r="C47" s="169"/>
-      <c r="D47" s="169"/>
-      <c r="E47" s="169"/>
-      <c r="F47" s="169"/>
-      <c r="G47" s="169"/>
-      <c r="H47" s="169"/>
-      <c r="I47" s="169"/>
-      <c r="J47" s="169"/>
-      <c r="K47" s="169"/>
-      <c r="L47" s="169"/>
-      <c r="M47" s="169"/>
-      <c r="N47" s="169"/>
-      <c r="O47" s="169"/>
-      <c r="P47" s="169"/>
-      <c r="Q47" s="169"/>
-      <c r="R47" s="169"/>
-      <c r="S47" s="169"/>
+      <c r="A47" s="166"/>
+      <c r="B47" s="166"/>
+      <c r="C47" s="166"/>
+      <c r="D47" s="166"/>
+      <c r="E47" s="166"/>
+      <c r="F47" s="166"/>
+      <c r="G47" s="166"/>
+      <c r="H47" s="166"/>
+      <c r="I47" s="166"/>
+      <c r="J47" s="166"/>
+      <c r="K47" s="166"/>
+      <c r="L47" s="166"/>
+      <c r="M47" s="166"/>
+      <c r="N47" s="166"/>
+      <c r="O47" s="166"/>
+      <c r="P47" s="166"/>
+      <c r="Q47" s="166"/>
+      <c r="R47" s="166"/>
+      <c r="S47" s="166"/>
       <c r="T47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="100"/>
-      <c r="B48" s="100"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="100"/>
-      <c r="E48" s="100"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="100"/>
-      <c r="J48" s="100"/>
-      <c r="K48" s="100"/>
-      <c r="L48" s="100"/>
-      <c r="M48" s="100"/>
-      <c r="N48" s="100"/>
-      <c r="O48" s="100"/>
-      <c r="P48" s="100"/>
-      <c r="Q48" s="100"/>
-      <c r="R48" s="100"/>
-      <c r="S48" s="100"/>
+      <c r="A48" s="96"/>
+      <c r="B48" s="96"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="96"/>
+      <c r="H48" s="96"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="96"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="96"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="96"/>
+      <c r="O48" s="96"/>
+      <c r="P48" s="96"/>
+      <c r="Q48" s="96"/>
+      <c r="R48" s="96"/>
+      <c r="S48" s="96"/>
       <c r="T48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="100"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
-      <c r="E49" s="100"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="100"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="100"/>
-      <c r="J49" s="100"/>
-      <c r="K49" s="100"/>
-      <c r="L49" s="100"/>
-      <c r="M49" s="100"/>
-      <c r="N49" s="100"/>
-      <c r="O49" s="100"/>
-      <c r="P49" s="100"/>
-      <c r="Q49" s="100"/>
-      <c r="R49" s="100"/>
-      <c r="S49" s="100"/>
+      <c r="A49" s="96"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="96"/>
+      <c r="H49" s="96"/>
+      <c r="I49" s="96"/>
+      <c r="J49" s="96"/>
+      <c r="K49" s="96"/>
+      <c r="L49" s="96"/>
+      <c r="M49" s="96"/>
+      <c r="N49" s="96"/>
+      <c r="O49" s="96"/>
+      <c r="P49" s="96"/>
+      <c r="Q49" s="96"/>
+      <c r="R49" s="96"/>
+      <c r="S49" s="96"/>
       <c r="T49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="100"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="100"/>
-      <c r="D50" s="100"/>
-      <c r="E50" s="100"/>
-      <c r="F50" s="100"/>
-      <c r="G50" s="100"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="100"/>
-      <c r="J50" s="100"/>
-      <c r="K50" s="100"/>
-      <c r="L50" s="100"/>
-      <c r="M50" s="100"/>
-      <c r="N50" s="100"/>
-      <c r="O50" s="100"/>
-      <c r="P50" s="100"/>
-      <c r="Q50" s="100"/>
-      <c r="R50" s="100"/>
-      <c r="S50" s="100"/>
+      <c r="A50" s="96"/>
+      <c r="B50" s="96"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="96"/>
+      <c r="K50" s="96"/>
+      <c r="L50" s="96"/>
+      <c r="M50" s="96"/>
+      <c r="N50" s="96"/>
+      <c r="O50" s="96"/>
+      <c r="P50" s="96"/>
+      <c r="Q50" s="96"/>
+      <c r="R50" s="96"/>
+      <c r="S50" s="96"/>
       <c r="T50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="100"/>
-      <c r="B51" s="100"/>
-      <c r="C51" s="100"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="100"/>
-      <c r="G51" s="100"/>
-      <c r="H51" s="100"/>
-      <c r="I51" s="100"/>
-      <c r="J51" s="100"/>
-      <c r="K51" s="100"/>
-      <c r="L51" s="100"/>
-      <c r="M51" s="100"/>
-      <c r="N51" s="100"/>
-      <c r="O51" s="100"/>
-      <c r="P51" s="100"/>
-      <c r="Q51" s="100"/>
-      <c r="R51" s="100"/>
-      <c r="S51" s="100"/>
+      <c r="A51" s="96"/>
+      <c r="B51" s="96"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="96"/>
+      <c r="E51" s="96"/>
+      <c r="F51" s="96"/>
+      <c r="G51" s="96"/>
+      <c r="H51" s="96"/>
+      <c r="I51" s="96"/>
+      <c r="J51" s="96"/>
+      <c r="K51" s="96"/>
+      <c r="L51" s="96"/>
+      <c r="M51" s="96"/>
+      <c r="N51" s="96"/>
+      <c r="O51" s="96"/>
+      <c r="P51" s="96"/>
+      <c r="Q51" s="96"/>
+      <c r="R51" s="96"/>
+      <c r="S51" s="96"/>
       <c r="T51" s="6"/>
     </row>
-    <row r="52" s="105" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="101"/>
-      <c r="B52" s="101"/>
-      <c r="C52" s="170" t="s">
+    <row r="52" s="101" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="97"/>
+      <c r="B52" s="97"/>
+      <c r="C52" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="170"/>
-      <c r="E52" s="170"/>
-      <c r="F52" s="170"/>
-      <c r="G52" s="170"/>
-      <c r="H52" s="170"/>
-      <c r="I52" s="170"/>
-      <c r="J52" s="171"/>
-      <c r="K52" s="172"/>
-      <c r="L52" s="173" t="s">
+      <c r="D52" s="167"/>
+      <c r="E52" s="167"/>
+      <c r="F52" s="167"/>
+      <c r="G52" s="167"/>
+      <c r="H52" s="167"/>
+      <c r="I52" s="167"/>
+      <c r="J52" s="168"/>
+      <c r="K52" s="169"/>
+      <c r="L52" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="M52" s="173"/>
-      <c r="N52" s="173"/>
-      <c r="O52" s="174"/>
-      <c r="P52" s="101"/>
-      <c r="Q52" s="101"/>
-      <c r="R52" s="101"/>
-      <c r="S52" s="101"/>
-      <c r="T52" s="101"/>
+      <c r="M52" s="170"/>
+      <c r="N52" s="170"/>
+      <c r="O52" s="171"/>
+      <c r="P52" s="97"/>
+      <c r="Q52" s="97"/>
+      <c r="R52" s="97"/>
+      <c r="S52" s="97"/>
+      <c r="T52" s="97"/>
     </row>
     <row r="53" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="175" t="s">
+      <c r="C53" s="172" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="175"/>
-      <c r="E53" s="176"/>
-      <c r="F53" s="176"/>
-      <c r="G53" s="176"/>
-      <c r="H53" s="176"/>
-      <c r="I53" s="175"/>
-      <c r="J53" s="171"/>
-      <c r="K53" s="177"/>
-      <c r="L53" s="178" t="s">
+      <c r="D53" s="172"/>
+      <c r="E53" s="173"/>
+      <c r="F53" s="173"/>
+      <c r="G53" s="173"/>
+      <c r="H53" s="173"/>
+      <c r="I53" s="172"/>
+      <c r="J53" s="168"/>
+      <c r="K53" s="174"/>
+      <c r="L53" s="175" t="s">
         <v>53</v>
       </c>
-      <c r="M53" s="178"/>
-      <c r="N53" s="178"/>
-      <c r="O53" s="176"/>
-      <c r="P53" s="176"/>
-      <c r="Q53" s="176"/>
+      <c r="M53" s="175"/>
+      <c r="N53" s="175"/>
+      <c r="O53" s="173"/>
+      <c r="P53" s="173"/>
+      <c r="Q53" s="173"/>
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="6"/>
@@ -5134,25 +5129,25 @@
     <row r="54" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="179" t="s">
+      <c r="C54" s="176" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="175"/>
-      <c r="E54" s="180"/>
-      <c r="F54" s="180"/>
-      <c r="G54" s="180"/>
-      <c r="H54" s="180"/>
-      <c r="I54" s="175"/>
-      <c r="J54" s="171"/>
-      <c r="K54" s="177"/>
-      <c r="L54" s="181" t="s">
+      <c r="D54" s="172"/>
+      <c r="E54" s="177"/>
+      <c r="F54" s="177"/>
+      <c r="G54" s="177"/>
+      <c r="H54" s="177"/>
+      <c r="I54" s="172"/>
+      <c r="J54" s="168"/>
+      <c r="K54" s="174"/>
+      <c r="L54" s="178" t="s">
         <v>54</v>
       </c>
-      <c r="M54" s="181"/>
-      <c r="N54" s="181"/>
-      <c r="O54" s="180"/>
-      <c r="P54" s="180"/>
-      <c r="Q54" s="180"/>
+      <c r="M54" s="178"/>
+      <c r="N54" s="178"/>
+      <c r="O54" s="177"/>
+      <c r="P54" s="177"/>
+      <c r="Q54" s="177"/>
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
       <c r="T54" s="6"/>
@@ -5160,25 +5155,25 @@
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="179" t="s">
+      <c r="C55" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="D55" s="175"/>
-      <c r="E55" s="180"/>
-      <c r="F55" s="180"/>
-      <c r="G55" s="180"/>
-      <c r="H55" s="180"/>
-      <c r="I55" s="175"/>
-      <c r="J55" s="171"/>
-      <c r="K55" s="177"/>
-      <c r="L55" s="181" t="s">
+      <c r="D55" s="172"/>
+      <c r="E55" s="177"/>
+      <c r="F55" s="177"/>
+      <c r="G55" s="177"/>
+      <c r="H55" s="177"/>
+      <c r="I55" s="172"/>
+      <c r="J55" s="168"/>
+      <c r="K55" s="174"/>
+      <c r="L55" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="M55" s="181"/>
-      <c r="N55" s="181"/>
-      <c r="O55" s="180"/>
-      <c r="P55" s="180"/>
-      <c r="Q55" s="180"/>
+      <c r="M55" s="178"/>
+      <c r="N55" s="178"/>
+      <c r="O55" s="177"/>
+      <c r="P55" s="177"/>
+      <c r="Q55" s="177"/>
       <c r="R55" s="6"/>
       <c r="S55" s="6"/>
       <c r="T55" s="6"/>
@@ -5186,25 +5181,25 @@
     <row r="56" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="179" t="s">
+      <c r="C56" s="176" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="175"/>
-      <c r="E56" s="180"/>
-      <c r="F56" s="180"/>
-      <c r="G56" s="180"/>
-      <c r="H56" s="180"/>
-      <c r="I56" s="175"/>
-      <c r="J56" s="171"/>
-      <c r="K56" s="177"/>
-      <c r="L56" s="181" t="s">
+      <c r="D56" s="172"/>
+      <c r="E56" s="177"/>
+      <c r="F56" s="177"/>
+      <c r="G56" s="177"/>
+      <c r="H56" s="177"/>
+      <c r="I56" s="172"/>
+      <c r="J56" s="168"/>
+      <c r="K56" s="174"/>
+      <c r="L56" s="178" t="s">
         <v>55</v>
       </c>
-      <c r="M56" s="181"/>
-      <c r="N56" s="181"/>
-      <c r="O56" s="180"/>
-      <c r="P56" s="180"/>
-      <c r="Q56" s="180"/>
+      <c r="M56" s="178"/>
+      <c r="N56" s="178"/>
+      <c r="O56" s="177"/>
+      <c r="P56" s="177"/>
+      <c r="Q56" s="177"/>
       <c r="R56" s="6"/>
       <c r="S56" s="6"/>
       <c r="T56" s="6"/>
@@ -5212,19 +5207,19 @@
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="123"/>
-      <c r="D57" s="123"/>
-      <c r="E57" s="123"/>
-      <c r="F57" s="123"/>
-      <c r="G57" s="123"/>
-      <c r="H57" s="123"/>
-      <c r="I57" s="123"/>
-      <c r="J57" s="182"/>
-      <c r="K57" s="182"/>
-      <c r="L57" s="123"/>
-      <c r="M57" s="123"/>
-      <c r="N57" s="123"/>
-      <c r="O57" s="123"/>
+      <c r="C57" s="120"/>
+      <c r="D57" s="120"/>
+      <c r="E57" s="120"/>
+      <c r="F57" s="120"/>
+      <c r="G57" s="120"/>
+      <c r="H57" s="120"/>
+      <c r="I57" s="120"/>
+      <c r="J57" s="179"/>
+      <c r="K57" s="179"/>
+      <c r="L57" s="120"/>
+      <c r="M57" s="120"/>
+      <c r="N57" s="120"/>
+      <c r="O57" s="120"/>
       <c r="P57" s="6"/>
       <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
@@ -5234,19 +5229,19 @@
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="123"/>
-      <c r="D58" s="123"/>
-      <c r="E58" s="123"/>
-      <c r="F58" s="123"/>
-      <c r="G58" s="123"/>
-      <c r="H58" s="123"/>
-      <c r="I58" s="123"/>
-      <c r="J58" s="123"/>
-      <c r="K58" s="123"/>
-      <c r="L58" s="123"/>
-      <c r="M58" s="123"/>
-      <c r="N58" s="123"/>
-      <c r="O58" s="123"/>
+      <c r="C58" s="120"/>
+      <c r="D58" s="120"/>
+      <c r="E58" s="120"/>
+      <c r="F58" s="120"/>
+      <c r="G58" s="120"/>
+      <c r="H58" s="120"/>
+      <c r="I58" s="120"/>
+      <c r="J58" s="120"/>
+      <c r="K58" s="120"/>
+      <c r="L58" s="120"/>
+      <c r="M58" s="120"/>
+      <c r="N58" s="120"/>
+      <c r="O58" s="120"/>
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
       <c r="R58" s="6"/>

</xml_diff>